<commit_message>
Bus Hire Test case added
</commit_message>
<xml_diff>
--- a/Resources/Test Data/TestDataRedBus.xlsx
+++ b/Resources/Test Data/TestDataRedBus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julianbenny\eclipse-workspace\Exit_test\Resources\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{264A7DF5-9026-4A93-B663-8689F12A7BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F36BF2-D3D9-4E0E-86BD-16A010BBB26B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="779" xr2:uid="{57D31B6C-5271-4BC7-9BCF-9A3C8BE0878B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="779" activeTab="3" xr2:uid="{57D31B6C-5271-4BC7-9BCF-9A3C8BE0878B}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchBusTestData" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="58">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -177,7 +177,40 @@
     <t>Outstation</t>
   </si>
   <si>
-    <t>User navigates to Bus Hire page from clicking Bus Hire button on HomePage and then fills out the query to view vehicles</t>
+    <t>Expected xpath of element</t>
+  </si>
+  <si>
+    <t>//div[contains(text(),'Fill Contact Details')]</t>
+  </si>
+  <si>
+    <t>Pickup</t>
+  </si>
+  <si>
+    <t>Destination</t>
+  </si>
+  <si>
+    <t>From Date and Time</t>
+  </si>
+  <si>
+    <t>To Date and Time</t>
+  </si>
+  <si>
+    <t>Num of passengers</t>
+  </si>
+  <si>
+    <t>Green Park, New Delhi, Delhi, India</t>
+  </si>
+  <si>
+    <t>Manali, Himachal Pradesh, India</t>
+  </si>
+  <si>
+    <t>12-08-2021-9:45 PM</t>
+  </si>
+  <si>
+    <t>17-08-2021-9:30 PM</t>
+  </si>
+  <si>
+    <t>User navigates to Bus Hire page from clicking Bus Hire button on HomePage, then selects outstation, and fills out the query to view vehicles</t>
   </si>
 </sst>
 </file>
@@ -562,7 +595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5866CE2D-7A03-41E5-A66E-D2508063588E}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -866,21 +899,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF50B6D1-3E5B-4BF8-8925-7BB963FC0DB8}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="44" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="54.08984375" customWidth="1"/>
-    <col min="4" max="4" width="35.81640625" customWidth="1"/>
+    <col min="2" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="54.08984375" customWidth="1"/>
+    <col min="9" max="9" width="35.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -888,21 +921,54 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>45</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
+      <c r="C2" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="D2" s="5" t="s">
-        <v>46</v>
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Homepage section test cases added. Test cases done.
</commit_message>
<xml_diff>
--- a/Resources/Test Data/TestDataRedBus.xlsx
+++ b/Resources/Test Data/TestDataRedBus.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julianbenny\eclipse-workspace\Exit_test\Resources\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F91C4B0C-7D3A-4F40-900C-C4E56CDAEF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396E506F-F00D-4E81-9DEC-4EF6F918151B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="779" activeTab="3" xr2:uid="{57D31B6C-5271-4BC7-9BCF-9A3C8BE0878B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="779" activeTab="4" xr2:uid="{57D31B6C-5271-4BC7-9BCF-9A3C8BE0878B}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchBusTestData" sheetId="1" r:id="rId1"/>
     <sheet name="HomePageTestData" sheetId="2" r:id="rId2"/>
     <sheet name="BookingData" sheetId="3" r:id="rId3"/>
     <sheet name="BusHireTestData" sheetId="4" r:id="rId4"/>
+    <sheet name="HomePageSectionTestData" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="82">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -174,9 +175,6 @@
     <t>Clicking on "Manage Booking" and then "EMAIL/SMS" to be taken to page for sending tickets via mail or sms</t>
   </si>
   <si>
-    <t>Outstation</t>
-  </si>
-  <si>
     <t>Expected xpath of element</t>
   </si>
   <si>
@@ -210,7 +208,151 @@
     <t>17-08-2021-9:30 PM</t>
   </si>
   <si>
-    <t>User navigates to Bus Hire page from clicking Bus Hire button on HomePage, then selects outstation, and fills out the query to view vehicles</t>
+    <t>Outstation Valid</t>
+  </si>
+  <si>
+    <t>//div[contains(text(),'Outstation')]</t>
+  </si>
+  <si>
+    <t>Outstation Invalid</t>
+  </si>
+  <si>
+    <t>Local Valid</t>
+  </si>
+  <si>
+    <t>Local Invalid</t>
+  </si>
+  <si>
+    <t>//div[contains(text(),'Local')]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">User navigates to Bus Hire page from clicking Bus Hire button on HomePage, then selects </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>outstation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, and fills out the query to view vehicles</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">User navigates to Bus Hire page from clicking Bus Hire button on HomePage, then selects </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>outstation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, and fills out incomplete queries and will be given prompt to fill all details</t>
+    </r>
+  </si>
+  <si>
+    <t>User navigates to Bus Hire page from clicking Bus Hire button on HomePage, then selects local, and fills out the query to view vehicles</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">User navigates to Bus Hire page from clicking Bus Hire button on HomePage, then selects </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>local</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, and fills out incomplete queries and will be given prompt to fill all details</t>
+    </r>
+  </si>
+  <si>
+    <t>Expected URL</t>
+  </si>
+  <si>
+    <t>Global Presence Section</t>
+  </si>
+  <si>
+    <t>https://www.redbus.sg/</t>
+  </si>
+  <si>
+    <t>User clicks on a singapore flag in global presence section and is redirected to singapore version of the website</t>
+  </si>
+  <si>
+    <t>https://www.redbus.in/online-booking/apsrtc</t>
+  </si>
+  <si>
+    <t>Different RTC's section</t>
+  </si>
+  <si>
+    <t>https://www.business-standard.com/article/companies/bs-annual-awards-saluting-the-spirit-of-entrepreneurship-114033100015_1.html</t>
+  </si>
+  <si>
+    <t>Award's Section</t>
+  </si>
+  <si>
+    <t>Operators Section</t>
+  </si>
+  <si>
+    <t>https://www.redbus.in/travels/kpn-travels-kpn</t>
+  </si>
+  <si>
+    <t>Our Partners Section</t>
+  </si>
+  <si>
+    <t>https://www.goibibo.com/</t>
+  </si>
+  <si>
+    <t>User clicks on Bussiness Standarad - Most Innovative Company(one of the award listed) in Awards and Recognition section</t>
+  </si>
+  <si>
+    <t>User clicks on KPN Travelers(one of the operator listed) in Top operators section</t>
+  </si>
+  <si>
+    <t>User clicks on APSRTC(one of the RTC listed) in Top RTC's section</t>
+  </si>
+  <si>
+    <t>User clicks on goibibo(one of the partner website listed) in Our Partner section</t>
   </si>
 </sst>
 </file>
@@ -717,7 +859,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:D6"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -899,10 +1041,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF50B6D1-3E5B-4BF8-8925-7BB963FC0DB8}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -921,22 +1063,22 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>6</v>
@@ -944,31 +1086,209 @@
     </row>
     <row r="2" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" t="s">
         <v>54</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>55</v>
-      </c>
-      <c r="F2" t="s">
-        <v>56</v>
       </c>
       <c r="G2">
         <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I2" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
         <v>57</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CF40F7A-C505-4B76-9685-183F9D671B96}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="44" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="54.08984375" customWidth="1"/>
+    <col min="4" max="4" width="35.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>